<commit_message>
Started building your app
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7f27a46b-5e12-4edd-bf3f-1219fdfc7add
</commit_message>
<xml_diff>
--- a/attached_assets/Complete_Real_Refineries_By_Region.xlsx
+++ b/attached_assets/Complete_Real_Refineries_By_Region.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIB PROGRAMS\PROJECT 2025\PROJECT IT TO DO MARCH 2025\SHIPBOAT BY JEAN\REFINERY EXCEL SHEETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIB PROGRAMS\PROJECT 2025\PROJECT IT TO DO MARCH 2025\SHIPBOAT BY JEAN\LIST EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Middle East" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="South Asia &amp; Oceania" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2764,7 +2765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4018,7 +4019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>